<commit_message>
add test for 100 insert images
</commit_message>
<xml_diff>
--- a/test/templates/test-insert-images.xlsx
+++ b/test/templates/test-insert-images.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\surveaexcel\NEWER\jduxlsx\test\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BB38D7-AB9D-40BE-A4D5-CB70F7739C82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091EB68F-6E6F-4788-8717-EFDFD0DF89D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init_rels" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>${image:imgB64}</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>${image:imgPath}</t>
+  </si>
+  <si>
+    <t>${test}</t>
   </si>
 </sst>
 </file>
@@ -442,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E55AD12-649B-4C2F-9DF3-E27C396ED218}">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,15 +758,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27A0DDC-A9A4-4806-B0A5-02020AC94F69}">
-  <dimension ref="B7"/>
+  <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
catch error if image does not exists
</commit_message>
<xml_diff>
--- a/test/templates/test-insert-images.xlsx
+++ b/test/templates/test-insert-images.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\surveaexcel\NEWER\jduxlsx\test\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091EB68F-6E6F-4788-8717-EFDFD0DF89D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48689D8-E58F-42D8-BE1D-08AFC4911241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="init_rels" sheetId="5" r:id="rId1"/>
     <sheet name="multi_test" sheetId="3" r:id="rId2"/>
     <sheet name="more_than_100" sheetId="6" r:id="rId3"/>
+    <sheet name="breaking_image" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>${image:imgB64}</t>
   </si>
@@ -466,7 +467,7 @@
   <dimension ref="B2:U32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27A0DDC-A9A4-4806-B0A5-02020AC94F69}">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -782,4 +783,29 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C3FF9A-844D-4DCD-8CB7-E306CCB201D8}">
+  <dimension ref="C5:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>